<commit_message>
embedding model 변경 실험 진행 중
</commit_message>
<xml_diff>
--- a/deuChatbot/test_automation/qna.xlsx
+++ b/deuChatbot/test_automation/qna.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minsu\Desktop\DeuChatbot\deuChatbot\test_automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCC4215-4CE8-4F7E-A86B-3CFC2A55F923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4CA0CD-BCF3-4290-9F6A-D23D8A56129E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{ABFFA3B5-2554-4543-A201-B6E726E2138D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ABFFA3B5-2554-4543-A201-B6E726E2138D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="297">
   <si>
     <t>질의</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -845,10 +846,6 @@
     <t>간호학과의 최종등록자 데이터를 기준으로 보면, 간호학과의 영어 등급 평균은 2.34이고, 수능 4개 영역 등급 평균은 3.37입니다. 
 따라서, 현재 정시 등급이 3.44이라면 간호학과에 합격하기 어려울 수 있습니다. 간호학과의 평균 등급보다 높은 성적을 가지고 있어야 합격 가능성이 높아집니다. 
 자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>간호학과 정시 성적 2.52 추합으로도 합격 안되겠죠...?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2005,6 +2002,14 @@
 8. 퇴실 .
 과정 중에서 면접은 면접위원 2~3인이 평가위원이 되어 수험생 1명을 대상으로 개별적으로 평가하며, 수험생의 답변 내용을 바탕으로 정성적이고 종합적으로 평가합니다. 또한 지원자별로 채용기업 심층면접이 이루어질 수 있으며, 이 과정에서도 면접위원 2~3인이 참여합니다 .
 추가적으로, 면접 시에는 개인신상정보에 대한 노출을 금지하며, 교복 착용도 금지됩니다 .</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>간호학과 정시 성적 2.52 추가 합격으로도 합격 안되겠죠...?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>간호학과 정시 성적이 3.7인데 정시 전형 합격할 수 있을까요?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2390,8 +2395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6B1BFF4-AFEB-47CA-A3A5-20AA54A6AED6}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2930,282 +2935,282 @@
     </row>
     <row r="67" spans="1:2" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
+        <v>295</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="132" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>296</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="132" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
+        <v>132</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="99" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
+        <v>134</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
+        <v>136</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
+        <v>138</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
+        <v>140</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="132" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
+        <v>142</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="165" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
+        <v>144</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="132" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
+        <v>146</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
+        <v>148</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="181.5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
+        <v>150</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="280.5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
+        <v>152</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
+        <v>154</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
+        <v>156</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="231" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
+        <v>158</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
+        <v>160</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="165" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
+        <v>162</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
+        <v>164</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
+        <v>166</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="165" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
+        <v>168</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="165" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
+        <v>170</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="247.5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
+        <v>172</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
+        <v>174</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="297" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
+        <v>176</v>
+      </c>
+      <c r="B91" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="132" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
+        <v>178</v>
+      </c>
+      <c r="B92" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
+        <v>180</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="363" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
+        <v>182</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="264" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
+        <v>184</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
+        <v>186</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
+        <v>188</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
+        <v>190</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
+        <v>192</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="231" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
+        <v>194</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="165" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
+        <v>196</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -3219,8 +3224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FA047E5-64A6-46F6-B6F2-6A9E7AD22C76}">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3233,7 +3238,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
@@ -3241,7 +3246,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
@@ -3249,7 +3254,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="181.5" x14ac:dyDescent="0.3">
@@ -3257,7 +3262,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="346.5" x14ac:dyDescent="0.3">
@@ -3265,7 +3270,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="181.5" x14ac:dyDescent="0.3">
@@ -3273,7 +3278,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="198" x14ac:dyDescent="0.3">
@@ -3281,7 +3286,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -3289,7 +3294,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3297,7 +3302,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3305,7 +3310,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
@@ -3313,7 +3318,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="181.5" x14ac:dyDescent="0.3">
@@ -3321,7 +3326,7 @@
         <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="132" x14ac:dyDescent="0.3">
@@ -3329,7 +3334,7 @@
         <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="214.5" x14ac:dyDescent="0.3">
@@ -3337,7 +3342,7 @@
         <v>28</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="165" x14ac:dyDescent="0.3">
@@ -3345,7 +3350,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3353,7 +3358,7 @@
         <v>32</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="115.5" x14ac:dyDescent="0.3">
@@ -3361,7 +3366,7 @@
         <v>34</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="396" x14ac:dyDescent="0.3">
@@ -3369,7 +3374,7 @@
         <v>36</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3377,7 +3382,7 @@
         <v>38</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="231" x14ac:dyDescent="0.3">
@@ -3385,7 +3390,7 @@
         <v>40</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="396" x14ac:dyDescent="0.3">
@@ -3393,7 +3398,7 @@
         <v>42</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="148.5" x14ac:dyDescent="0.3">
@@ -3401,7 +3406,7 @@
         <v>44</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3409,7 +3414,7 @@
         <v>46</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="165" x14ac:dyDescent="0.3">
@@ -3417,7 +3422,7 @@
         <v>48</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3425,7 +3430,7 @@
         <v>50</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="214.5" x14ac:dyDescent="0.3">
@@ -3433,7 +3438,7 @@
         <v>52</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="264" x14ac:dyDescent="0.3">
@@ -3441,7 +3446,7 @@
         <v>54</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="346.5" x14ac:dyDescent="0.3">
@@ -3449,7 +3454,7 @@
         <v>56</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3457,7 +3462,7 @@
         <v>58</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3465,7 +3470,7 @@
         <v>60</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3473,7 +3478,7 @@
         <v>62</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="231" x14ac:dyDescent="0.3">
@@ -3481,7 +3486,7 @@
         <v>64</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3489,7 +3494,7 @@
         <v>66</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3497,7 +3502,7 @@
         <v>68</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3505,7 +3510,7 @@
         <v>70</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="165" x14ac:dyDescent="0.3">
@@ -3513,7 +3518,7 @@
         <v>72</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="297" x14ac:dyDescent="0.3">
@@ -3521,7 +3526,7 @@
         <v>74</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="330" x14ac:dyDescent="0.3">
@@ -3529,7 +3534,7 @@
         <v>76</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="132" x14ac:dyDescent="0.3">
@@ -3537,7 +3542,7 @@
         <v>78</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="280.5" x14ac:dyDescent="0.3">
@@ -3545,7 +3550,7 @@
         <v>80</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3553,7 +3558,7 @@
         <v>82</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3561,7 +3566,7 @@
         <v>84</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="165" x14ac:dyDescent="0.3">
@@ -3569,7 +3574,7 @@
         <v>86</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="181.5" x14ac:dyDescent="0.3">
@@ -3577,7 +3582,7 @@
         <v>88</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3585,7 +3590,7 @@
         <v>90</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="363" x14ac:dyDescent="0.3">
@@ -3593,7 +3598,7 @@
         <v>92</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="115.5" x14ac:dyDescent="0.3">
@@ -3601,7 +3606,7 @@
         <v>93</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="115.5" x14ac:dyDescent="0.3">
@@ -3609,7 +3614,7 @@
         <v>95</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3617,7 +3622,7 @@
         <v>97</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3625,7 +3630,7 @@
         <v>99</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3633,7 +3638,7 @@
         <v>101</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3641,7 +3646,7 @@
         <v>103</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3649,7 +3654,7 @@
         <v>105</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="363" x14ac:dyDescent="0.3">
@@ -3657,7 +3662,7 @@
         <v>107</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3665,7 +3670,7 @@
         <v>109</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="264" x14ac:dyDescent="0.3">
@@ -3673,7 +3678,7 @@
         <v>111</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3681,7 +3686,7 @@
         <v>113</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3689,7 +3694,7 @@
         <v>115</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3697,7 +3702,7 @@
         <v>117</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3705,7 +3710,7 @@
         <v>119</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3713,7 +3718,7 @@
         <v>121</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3721,7 +3726,7 @@
         <v>123</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3729,7 +3734,7 @@
         <v>125</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3737,7 +3742,7 @@
         <v>127</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
@@ -3745,287 +3750,287 @@
         <v>129</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>131</v>
+        <v>295</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="313.5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="313.5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="231" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -4033,4 +4038,828 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CC76CEC-5492-4766-A2B7-0246B1CCAFD5}">
+  <dimension ref="A1:B101"/>
+  <sheetViews>
+    <sheetView topLeftCell="A101" workbookViewId="0">
+      <selection sqref="A1:B101"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="148.5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="181.5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="181.5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="231" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="99" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="132" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="214.5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="66" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="198" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="330" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="132" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="181.5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="165" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="132" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="297" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="346.5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="379.5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="280.5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="297" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="297" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="198" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="379.5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="165" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="165" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>93</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="346.5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>95</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="231" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>99</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>101</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>103</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>105</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>107</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="280.5" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>109</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>111</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>113</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>115</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="297" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>117</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>119</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>121</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>123</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>125</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>127</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>129</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>295</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>296</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>132</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>134</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>136</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>138</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>140</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>142</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>144</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>146</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>148</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>150</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>152</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>154</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>156</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>158</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>160</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>162</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>164</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>166</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>168</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>170</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>172</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>174</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>176</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>178</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>180</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>182</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>184</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>186</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>188</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>190</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>192</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>194</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>196</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
experiment: 실험에 사용될 임베딩 종류 추가 - 현재 HuggingFace(12), OpenAI(3)
</commit_message>
<xml_diff>
--- a/deuChatbot/test_automation/qna.xlsx
+++ b/deuChatbot/test_automation/qna.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minsu\Desktop\DeuChatbot\deuChatbot\test_automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4CA0CD-BCF3-4290-9F6A-D23D8A56129E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E068AA2-DD07-44EA-8336-815B3BCA7505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ABFFA3B5-2554-4543-A201-B6E726E2138D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="317">
   <si>
     <t>질의</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2010,6 +2010,86 @@
   </si>
   <si>
     <t>간호학과 정시 성적이 3.7인데 정시 전형 합격할 수 있을까요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평생학습자전형에 대해 알려줘.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평생학습자전형 지원자격은?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>실기고사는 어디로 가면 되나요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>체육학과의 실기고사는 어디로 가면 되나요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023학년도 경찰행정학과 수시모집 결과는?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동의대학교 정시 일정에 대해 설명해주세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동의대학교 정시 모집 일정에 대해 설명해주세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>농어촌학생전형으로 지원 시 제출해야할 서류는?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>농어촌학생전형으로 지원 시 12년 과정이 제출해야할 서류는?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e비즈니스학전공 예비38번 이정도면 예비합격 가능할지 궁금합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>간호학과 - 동의대식 정시 성적 3.44인데 마지막으로 문 닫고 들어 올 가능성도 없나요??</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동의대학교 e비즈니스학과 정시 등급 5.3이면 최초합 가능성 있을까?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>간호학과 정시 성적 2.52 추가 합격으로도 합격 안되겠죠?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>간호학과 정시 성적이 2.58인데 정시 전형 합격할 수 있을까요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경영정보학과 정시 성적 3.75 인데 최초합으로 가능할까용?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정시 성적으로 4.75 나오는데 가능할까요?? 그리고 유아교육학과는 이 성적으로 어렵겠죠 ?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제가 동의대 정시 환산등급이 4.16인데 보육가정상담학과 일반학생전형으로 추합까지 생각해서 합격이 될까요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동의대 수능 정시 산출로 4.5나왔는데 추가모집이든 해서 들어갈수 있을까요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동의대학교 신소재 공학부 합격 가능할까요? 정시등급은 몇 인가여 신소재 학과는?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제가 동의대학교 정시 표준점수가 447점으로 환산되는데 작년 신소재공학과 표점이 447점보다 1점 정도 위더라구요 (최종 평균)가능성은 있늘까요??</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2395,8 +2475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6B1BFF4-AFEB-47CA-A3A5-20AA54A6AED6}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2751,7 +2831,7 @@
     </row>
     <row r="44" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>86</v>
+        <v>297</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>87</v>
@@ -2759,7 +2839,7 @@
     </row>
     <row r="45" spans="1:2" ht="99" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>88</v>
+        <v>298</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>89</v>
@@ -2767,7 +2847,7 @@
     </row>
     <row r="46" spans="1:2" ht="33" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>90</v>
+        <v>299</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>91</v>
@@ -2775,7 +2855,7 @@
     </row>
     <row r="47" spans="1:2" ht="33" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>92</v>
+        <v>300</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>91</v>
@@ -2791,7 +2871,7 @@
     </row>
     <row r="49" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>95</v>
+        <v>301</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>96</v>
@@ -2815,7 +2895,7 @@
     </row>
     <row r="52" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>101</v>
+        <v>302</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>102</v>
@@ -2823,7 +2903,7 @@
     </row>
     <row r="53" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>103</v>
+        <v>303</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>104</v>
@@ -2863,7 +2943,7 @@
     </row>
     <row r="58" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>113</v>
+        <v>304</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>114</v>
@@ -2871,7 +2951,7 @@
     </row>
     <row r="59" spans="1:2" ht="247.5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>115</v>
+        <v>305</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>116</v>
@@ -2911,7 +2991,7 @@
     </row>
     <row r="64" spans="1:2" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>125</v>
+        <v>308</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>126</v>
@@ -2919,7 +2999,7 @@
     </row>
     <row r="65" spans="1:2" ht="99" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>127</v>
+        <v>306</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>128</v>
@@ -2927,7 +3007,7 @@
     </row>
     <row r="66" spans="1:2" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>129</v>
+        <v>307</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>130</v>
@@ -2935,7 +3015,7 @@
     </row>
     <row r="67" spans="1:2" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>295</v>
+        <v>309</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>131</v>
@@ -2951,7 +3031,7 @@
     </row>
     <row r="69" spans="1:2" ht="132" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>132</v>
+        <v>310</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>133</v>
@@ -2975,7 +3055,7 @@
     </row>
     <row r="72" spans="1:2" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>138</v>
+        <v>311</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>139</v>
@@ -3063,7 +3143,7 @@
     </row>
     <row r="83" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>160</v>
+        <v>312</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>161</v>
@@ -3071,7 +3151,7 @@
     </row>
     <row r="84" spans="1:2" ht="165" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>162</v>
+        <v>313</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>163</v>
@@ -3127,7 +3207,7 @@
     </row>
     <row r="91" spans="1:2" ht="297" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>176</v>
+        <v>314</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>177</v>
@@ -3135,7 +3215,7 @@
     </row>
     <row r="92" spans="1:2" ht="132" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>178</v>
+        <v>315</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>179</v>
@@ -3143,7 +3223,7 @@
     </row>
     <row r="93" spans="1:2" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>180</v>
+        <v>316</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>181</v>

</xml_diff>